<commit_message>
add test to login page
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC01_Login/TC01_Login_TestCase.xlsx
+++ b/Documents/1_TestCases/TC01_Login/TC01_Login_TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC01_Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DE29FB-7F0D-4129-8AB3-3C210B593CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAD60A1-BF76-4366-9B71-145BAE79D4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="329" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>Title</t>
   </si>
@@ -275,6 +275,9 @@
 - Facebook: https://www.facebook.com/OrangeHRM/
 - Twitter: https://x.com/orangehrm?lang=en
 - Youtube: https://www.youtube.com/c/OrangeHRMInc</t>
+  </si>
+  <si>
+    <t>Username field should be case insensitive.</t>
   </si>
 </sst>
 </file>
@@ -341,33 +344,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="38">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -554,15 +546,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -601,51 +584,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7257DFA7-01A6-4206-A23E-FB97593526F5}" name="Table7" displayName="Table7" ref="B2:I498" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7257DFA7-01A6-4206-A23E-FB97593526F5}" name="Table7" displayName="Table7" ref="B2:I498" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="B2:I498" xr:uid="{7257DFA7-01A6-4206-A23E-FB97593526F5}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8A48E4F0-6353-4B65-A8AA-A9F47744DFE9}" name="Test ID" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{C69B3631-9235-49D5-835A-460725D8F78E}" name="Title" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{FE303652-83BF-4573-BA20-427DA11D17C1}" name="Preconditions" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{A40F81CC-1AF0-48A1-A33A-883B55562B5E}" name="Test Steps" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{8A0ED7D9-F5B9-4D05-BDCD-AA18270243C5}" name="Expected Result" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{95F71F64-2115-4AB0-9059-152D26C46054}" name="Actual Result" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{901AD4F1-00E9-4B40-B687-A2140805F52D}" name="Notes" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{324B268D-5B58-47CB-AE05-5CFCA1EC0FCA}" name="Status" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{8A48E4F0-6353-4B65-A8AA-A9F47744DFE9}" name="Test ID" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{C69B3631-9235-49D5-835A-460725D8F78E}" name="Title" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{FE303652-83BF-4573-BA20-427DA11D17C1}" name="Preconditions" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{A40F81CC-1AF0-48A1-A33A-883B55562B5E}" name="Test Steps" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{8A0ED7D9-F5B9-4D05-BDCD-AA18270243C5}" name="Expected Result" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{95F71F64-2115-4AB0-9059-152D26C46054}" name="Actual Result" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{901AD4F1-00E9-4B40-B687-A2140805F52D}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{324B268D-5B58-47CB-AE05-5CFCA1EC0FCA}" name="Status" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{82B24A36-2447-4983-855A-AAB06659A179}" name="Table723" displayName="Table723" ref="B2:I498" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{82B24A36-2447-4983-855A-AAB06659A179}" name="Table723" displayName="Table723" ref="B2:I498" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="B2:I498" xr:uid="{82B24A36-2447-4983-855A-AAB06659A179}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A30CC88D-34C6-4549-9F95-256E87B9A556}" name="Test ID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D2291B80-E052-4E74-8B2A-5348F0A9A3D3}" name="Title" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{FC5C0E58-90FA-4751-A365-F0E42870FF91}" name="Preconditions" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{50947D0F-3DB7-4C12-8D4C-04394E1E90D0}" name="Test Steps" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{C23F293D-C3E7-4952-A142-93091D0BBA3E}" name="Expected Result" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{E4077C5A-BC87-41F6-8F95-FA84454DECA1}" name="Actual Result" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{04A9F52E-CEAC-42B0-9466-31539452F358}" name="Notes" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{57C8C03B-F3D8-466A-ABA1-EB9E303A0381}" name="Status" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{A30CC88D-34C6-4549-9F95-256E87B9A556}" name="Test ID" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{D2291B80-E052-4E74-8B2A-5348F0A9A3D3}" name="Title" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{FC5C0E58-90FA-4751-A365-F0E42870FF91}" name="Preconditions" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{50947D0F-3DB7-4C12-8D4C-04394E1E90D0}" name="Test Steps" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{C23F293D-C3E7-4952-A142-93091D0BBA3E}" name="Expected Result" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{E4077C5A-BC87-41F6-8F95-FA84454DECA1}" name="Actual Result" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{04A9F52E-CEAC-42B0-9466-31539452F358}" name="Notes" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{57C8C03B-F3D8-466A-ABA1-EB9E303A0381}" name="Status" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1664E53-4BFC-46B7-A6E6-AE28B3F96B21}" name="Table72" displayName="Table72" ref="B2:I498" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1664E53-4BFC-46B7-A6E6-AE28B3F96B21}" name="Table72" displayName="Table72" ref="B2:I498" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B2:I498" xr:uid="{F1664E53-4BFC-46B7-A6E6-AE28B3F96B21}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C6AD6E72-D619-4F7A-A1B4-F56CA301BF0F}" name="Test ID" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{24DDBA72-E28E-474C-B5E1-AE041F298912}" name="Title" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{A274BD55-FA63-4D64-A320-6DFA74009ED5}" name="Preconditions" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{D075414E-2C83-4F70-8A30-EC33A8A439EA}" name="Test Steps" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{1C6D04CC-10B8-42A6-BC86-F64F2E5B8658}" name="Expected Result" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{799D8859-E4C3-464E-84FE-5F0D5D814832}" name="Actual Result" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{BD31614B-51C2-43FA-806D-187A71AF37CD}" name="Notes" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{D97C39C9-9A52-4956-93D9-99A7906A6516}" name="Status" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{C6AD6E72-D619-4F7A-A1B4-F56CA301BF0F}" name="Test ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{24DDBA72-E28E-474C-B5E1-AE041F298912}" name="Title" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{A274BD55-FA63-4D64-A320-6DFA74009ED5}" name="Preconditions" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{D075414E-2C83-4F70-8A30-EC33A8A439EA}" name="Test Steps" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{1C6D04CC-10B8-42A6-BC86-F64F2E5B8658}" name="Expected Result" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{799D8859-E4C3-464E-84FE-5F0D5D814832}" name="Actual Result" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{BD31614B-51C2-43FA-806D-187A71AF37CD}" name="Notes" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D97C39C9-9A52-4956-93D9-99A7906A6516}" name="Status" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -914,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I498"/>
+  <dimension ref="B2:I498"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +917,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -960,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>67</v>
       </c>
@@ -983,7 +966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>66</v>
       </c>
@@ -1006,7 +989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>65</v>
       </c>
@@ -1029,7 +1012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>64</v>
       </c>
@@ -1052,7 +1035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>63</v>
       </c>
@@ -1075,7 +1058,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>62</v>
       </c>
@@ -1098,7 +1081,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>61</v>
       </c>
@@ -1121,7 +1104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>60</v>
       </c>
@@ -1144,7 +1127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>59</v>
       </c>
@@ -1167,8 +1150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    <row r="12" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1182,13 +1164,14 @@
         <v>37</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>58</v>
       </c>
@@ -1205,9 +1188,11 @@
         <v>41</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="H13" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>72</v>
       </c>
@@ -1223,19 +1208,22 @@
       <c r="F14" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="H14" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1245,7 +1233,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1255,7 +1243,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1265,7 +1253,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -2707,11 +2695,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H1 I2:I11 H499:H1048576 I14:I498">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="H1 I2:I11 I14:I498 H499:H1048576">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2730,7 +2718,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0E1303-6B42-4513-AE24-731061DAA27B}">
-  <dimension ref="A2:I498"/>
+  <dimension ref="B2:I498"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -2750,7 +2738,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2776,7 +2764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>55</v>
       </c>
@@ -2791,7 +2779,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>56</v>
       </c>
@@ -2803,42 +2791,40 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
@@ -4288,20 +4274,20 @@
       <c r="I498" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1 I2 H499:H1048576 I5:I498">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="H1 H499:H1048576">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I4">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I3)))</formula>
+  <conditionalFormatting sqref="I2:I498">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I3)))</formula>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4318,7 +4304,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3006AF6B-5FD9-438F-BBCE-C610C3551B37}">
-  <dimension ref="A2:I498"/>
+  <dimension ref="B2:I498"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -4338,7 +4324,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4364,7 +4350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>68</v>
       </c>
@@ -4385,7 +4371,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>69</v>
       </c>
@@ -4406,7 +4392,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>70</v>
       </c>
@@ -4427,7 +4413,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
@@ -4448,36 +4434,34 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
@@ -5928,10 +5912,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 I2:I498 H499:H1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add login accessibility test, run axe-core analysis and documented in docs/results/login_accessibility
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC01_Login/TC01_Login_TestCase.xlsx
+++ b/Documents/1_TestCases/TC01_Login/TC01_Login_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC01_Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAD60A1-BF76-4366-9B71-145BAE79D4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130DCF2B-EDA4-45D5-998E-CCF83DBF0453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="329" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="329" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Title</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>Username field should be case insensitive.</t>
+  </si>
+  <si>
+    <t>Outlines are visible.</t>
+  </si>
+  <si>
+    <t>The login is successful with only keyboard.</t>
+  </si>
+  <si>
+    <t>Login Page can be zoomed in/out for 75% without breaking the ui.</t>
   </si>
 </sst>
 </file>
@@ -352,15 +361,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -546,6 +546,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -592,43 +601,43 @@
     <tableColumn id="3" xr3:uid="{FE303652-83BF-4573-BA20-427DA11D17C1}" name="Preconditions" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{A40F81CC-1AF0-48A1-A33A-883B55562B5E}" name="Test Steps" dataDxfId="32"/>
     <tableColumn id="5" xr3:uid="{8A0ED7D9-F5B9-4D05-BDCD-AA18270243C5}" name="Expected Result" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{95F71F64-2115-4AB0-9059-152D26C46054}" name="Actual Result" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{901AD4F1-00E9-4B40-B687-A2140805F52D}" name="Notes" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{324B268D-5B58-47CB-AE05-5CFCA1EC0FCA}" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{95F71F64-2115-4AB0-9059-152D26C46054}" name="Actual Result" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{901AD4F1-00E9-4B40-B687-A2140805F52D}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{324B268D-5B58-47CB-AE05-5CFCA1EC0FCA}" name="Status" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{82B24A36-2447-4983-855A-AAB06659A179}" name="Table723" displayName="Table723" ref="B2:I498" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{82B24A36-2447-4983-855A-AAB06659A179}" name="Table723" displayName="Table723" ref="B2:I498" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="B2:I498" xr:uid="{82B24A36-2447-4983-855A-AAB06659A179}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A30CC88D-34C6-4549-9F95-256E87B9A556}" name="Test ID" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{D2291B80-E052-4E74-8B2A-5348F0A9A3D3}" name="Title" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{FC5C0E58-90FA-4751-A365-F0E42870FF91}" name="Preconditions" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{50947D0F-3DB7-4C12-8D4C-04394E1E90D0}" name="Test Steps" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{C23F293D-C3E7-4952-A142-93091D0BBA3E}" name="Expected Result" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{E4077C5A-BC87-41F6-8F95-FA84454DECA1}" name="Actual Result" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{04A9F52E-CEAC-42B0-9466-31539452F358}" name="Notes" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{57C8C03B-F3D8-466A-ABA1-EB9E303A0381}" name="Status" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{A30CC88D-34C6-4549-9F95-256E87B9A556}" name="Test ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{D2291B80-E052-4E74-8B2A-5348F0A9A3D3}" name="Title" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{FC5C0E58-90FA-4751-A365-F0E42870FF91}" name="Preconditions" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{50947D0F-3DB7-4C12-8D4C-04394E1E90D0}" name="Test Steps" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{C23F293D-C3E7-4952-A142-93091D0BBA3E}" name="Expected Result" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{E4077C5A-BC87-41F6-8F95-FA84454DECA1}" name="Actual Result" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{04A9F52E-CEAC-42B0-9466-31539452F358}" name="Notes" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{57C8C03B-F3D8-466A-ABA1-EB9E303A0381}" name="Status" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1664E53-4BFC-46B7-A6E6-AE28B3F96B21}" name="Table72" displayName="Table72" ref="B2:I498" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1664E53-4BFC-46B7-A6E6-AE28B3F96B21}" name="Table72" displayName="Table72" ref="B2:I498" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="B2:I498" xr:uid="{F1664E53-4BFC-46B7-A6E6-AE28B3F96B21}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C6AD6E72-D619-4F7A-A1B4-F56CA301BF0F}" name="Test ID" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{24DDBA72-E28E-474C-B5E1-AE041F298912}" name="Title" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{A274BD55-FA63-4D64-A320-6DFA74009ED5}" name="Preconditions" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{D075414E-2C83-4F70-8A30-EC33A8A439EA}" name="Test Steps" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{1C6D04CC-10B8-42A6-BC86-F64F2E5B8658}" name="Expected Result" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{799D8859-E4C3-464E-84FE-5F0D5D814832}" name="Actual Result" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{BD31614B-51C2-43FA-806D-187A71AF37CD}" name="Notes" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{D97C39C9-9A52-4956-93D9-99A7906A6516}" name="Status" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{C6AD6E72-D619-4F7A-A1B4-F56CA301BF0F}" name="Test ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{24DDBA72-E28E-474C-B5E1-AE041F298912}" name="Title" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A274BD55-FA63-4D64-A320-6DFA74009ED5}" name="Preconditions" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{D075414E-2C83-4F70-8A30-EC33A8A439EA}" name="Test Steps" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{1C6D04CC-10B8-42A6-BC86-F64F2E5B8658}" name="Expected Result" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{799D8859-E4C3-464E-84FE-5F0D5D814832}" name="Actual Result" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{BD31614B-51C2-43FA-806D-187A71AF37CD}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{D97C39C9-9A52-4956-93D9-99A7906A6516}" name="Status" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -899,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,6 +1179,9 @@
       <c r="H12" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I12" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
@@ -1191,6 +1203,9 @@
       <c r="H13" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I13" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
@@ -1211,7 +1226,9 @@
       <c r="H14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
@@ -2695,16 +2712,16 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H1 I2:I11 I14:I498 H499:H1048576">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="H1 H499:H1048576 I2:I498">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I11 I14:I498" xr:uid="{8705CB75-3265-4505-B20A-B47F34467CE5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I498" xr:uid="{8705CB75-3265-4505-B20A-B47F34467CE5}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4275,18 +4292,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 H499:H1048576">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I498">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4306,7 +4323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3006AF6B-5FD9-438F-BBCE-C610C3551B37}">
   <dimension ref="B2:I498"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -4318,7 +4335,7 @@
     <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="54.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="41.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33" style="3" customWidth="1"/>
     <col min="8" max="8" width="38.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
@@ -4366,10 +4383,15 @@
       <c r="F3" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="H3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -4387,10 +4409,15 @@
       <c r="F4" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -4429,10 +4456,15 @@
       <c r="F6" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="3"/>
@@ -5912,10 +5944,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1 I2:I498 H499:H1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>